<commit_message>
Adding scrrenshots of test results from Genkins, Extend report , TestNG results
</commit_message>
<xml_diff>
--- a/Data/DataSheet.xlsx
+++ b/Data/DataSheet.xlsx
@@ -101,46 +101,46 @@
     <t>Pass scenario</t>
   </si>
   <si>
-    <t>Tamilarasa</t>
+    <t>Metalion</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>Metalion11@gmail.com</t>
+  </si>
+  <si>
+    <t>WeAreBest</t>
+  </si>
+  <si>
+    <t>8678003411</t>
+  </si>
+  <si>
+    <t>allCorrect</t>
+  </si>
+  <si>
+    <t>nil</t>
+  </si>
+  <si>
+    <t>Neweter</t>
+  </si>
+  <si>
+    <t>kocher155@gmail.com</t>
+  </si>
+  <si>
+    <t>7809933452</t>
+  </si>
+  <si>
+    <t>existingEmail</t>
+  </si>
+  <si>
+    <t>Metaduck</t>
   </si>
   <si>
     <t>pandiyan</t>
   </si>
   <si>
-    <t>Tamilarasapandiyan111@gmail.com</t>
-  </si>
-  <si>
-    <t>WeAreBest</t>
-  </si>
-  <si>
-    <t>8678003499</t>
-  </si>
-  <si>
-    <t>allCorrect</t>
-  </si>
-  <si>
-    <t>nil</t>
-  </si>
-  <si>
-    <t>Neweter</t>
-  </si>
-  <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>kocher155@gmail.com</t>
-  </si>
-  <si>
-    <t>7809933452</t>
-  </si>
-  <si>
-    <t>existingEmail</t>
-  </si>
-  <si>
-    <t>Tamilselvi</t>
-  </si>
-  <si>
-    <t>Tamilselvipandiyan2220@gmail.com</t>
+    <t>Metaduck22@gmail.com</t>
   </si>
   <si>
     <t>8096544239</t>
@@ -242,13 +242,13 @@
     <t>wrongConfirmPassword</t>
   </si>
   <si>
-    <t>Chidambaram</t>
+    <t>Metamonkey</t>
   </si>
   <si>
     <t>pillai</t>
   </si>
   <si>
-    <t>Chidambarampillai333@gmail.com</t>
+    <t>Metamonkey33@gmail.com</t>
   </si>
   <si>
     <t>0000000000</t>
@@ -262,10 +262,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -301,7 +301,53 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -315,34 +361,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -354,6 +384,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,7 +415,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -375,58 +427,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -437,187 +437,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -628,6 +628,24 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -642,6 +660,21 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -678,6 +711,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -686,189 +728,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1457,10 +1457,10 @@
         <v>35</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>37</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>31</v>
@@ -1469,13 +1469,13 @@
         <v>31</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>34</v>
@@ -1483,10 +1483,10 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>41</v>
@@ -1515,7 +1515,7 @@
         <v>44</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>45</v>
@@ -1544,7 +1544,7 @@
         <v>50</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>51</v>
@@ -1573,7 +1573,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>56</v>
@@ -1602,7 +1602,7 @@
         <v>60</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>61</v>
@@ -1631,7 +1631,7 @@
         <v>65</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>66</v>
@@ -1733,15 +1733,15 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" display="kocher155@gmail.com" tooltip="mailto:kocher155@gmail.com"/>
-    <hyperlink ref="C4" r:id="rId2" display="Tamilselvipandiyan2220@gmail.com" tooltip="mailto:Tamilselvipandiyan2220@gmail.com"/>
+    <hyperlink ref="C4" r:id="rId2" display="Metaduck22@gmail.com" tooltip="mailto:Metaduck22@gmail.com"/>
     <hyperlink ref="C5" r:id="rId3" display="Swettter0033@gmail.com" tooltip="mailto:Swettter0033@gmail.com"/>
     <hyperlink ref="C6" r:id="rId4" display="Mosterer3156@gmail.com" tooltip="mailto:Mosterer3156@gmail.com"/>
     <hyperlink ref="C7" r:id="rId5" display="Posterer1996@gmail.com" tooltip="mailto:Posterer1996@gmail.com"/>
     <hyperlink ref="C8" r:id="rId6" display="Forsterr2211@gmail.com" tooltip="mailto:Forsterr2211@gmail.com"/>
     <hyperlink ref="C9" r:id="rId7" display="Pensylasster7878@gmail.com" tooltip="mailto:Pensylasster7878@gmail.com"/>
     <hyperlink ref="C11" r:id="rId8" display="Dexteerbab1233@gmail.com"/>
-    <hyperlink ref="C12" r:id="rId9" display="Chidambarampillai333@gmail.com" tooltip="mailto:Chidambarampillai333@gmail.com"/>
-    <hyperlink ref="C2" r:id="rId10" display="Tamilarasapandiyan111@gmail.com" tooltip="mailto:Tamilarasapandiyan111@gmail.com"/>
+    <hyperlink ref="C12" r:id="rId9" display="Metamonkey33@gmail.com" tooltip="mailto:Metamonkey33@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId10" display="Metalion11@gmail.com" tooltip="mailto:Metalion11@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Adding passed test case screenshots with Read me file added to project
</commit_message>
<xml_diff>
--- a/Data/DataSheet.xlsx
+++ b/Data/DataSheet.xlsx
@@ -263,9 +263,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -301,7 +301,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -315,10 +323,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -330,6 +355,50 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -338,30 +407,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -370,58 +422,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -437,66 +437,180 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -504,120 +618,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -628,6 +628,32 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -649,21 +675,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -675,21 +686,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -718,13 +714,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -733,142 +733,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1240,7 +1240,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="3"/>
@@ -1377,7 +1377,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:I12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>

</xml_diff>